<commit_message>
all things related to countries
</commit_message>
<xml_diff>
--- a/data/Eksklusionslister/Akademiker Pension_eksklusionsliste.xlsx
+++ b/data/Eksklusionslister/Akademiker Pension_eksklusionsliste.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Anja\Documents\Python_projekter\kommune_investering\data\Eksklusionslister\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://gravercentret-my.sharepoint.com/personal/anja_gravercentret_dk/Documents/Dokumenter/Python_projekter/kommune_investering/data/Eksklusionslister/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{467D6647-A440-41EE-A299-57804ABFCA68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{B848B545-B42C-4FA7-95B2-4C6549080FB3}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{B848B545-B42C-4FA7-95B2-4C6549080FB3}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -821,16 +821,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF8BBBFE-AA4A-4E8A-BC5C-E7F63B19A243}">
   <dimension ref="A1:B126"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A113" workbookViewId="0">
-      <selection activeCell="A129" sqref="A129"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="34.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -838,7 +838,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -846,7 +846,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -854,7 +854,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
@@ -862,7 +862,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
@@ -870,7 +870,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
@@ -878,7 +878,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
@@ -886,7 +886,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>8</v>
       </c>
@@ -894,7 +894,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>9</v>
       </c>
@@ -902,7 +902,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>10</v>
       </c>
@@ -910,7 +910,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>11</v>
       </c>
@@ -918,7 +918,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>12</v>
       </c>
@@ -926,7 +926,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>13</v>
       </c>
@@ -934,7 +934,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>14</v>
       </c>
@@ -942,7 +942,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>15</v>
       </c>
@@ -950,7 +950,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>16</v>
       </c>
@@ -958,7 +958,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>17</v>
       </c>
@@ -966,7 +966,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>18</v>
       </c>
@@ -974,7 +974,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>19</v>
       </c>
@@ -982,7 +982,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>20</v>
       </c>
@@ -990,7 +990,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>21</v>
       </c>
@@ -998,7 +998,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>22</v>
       </c>
@@ -1006,7 +1006,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="23" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>23</v>
       </c>
@@ -1014,7 +1014,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>24</v>
       </c>
@@ -1022,7 +1022,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>25</v>
       </c>
@@ -1030,7 +1030,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>27</v>
       </c>
@@ -1038,7 +1038,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>28</v>
       </c>
@@ -1046,7 +1046,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>29</v>
       </c>
@@ -1054,7 +1054,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>30</v>
       </c>
@@ -1062,7 +1062,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>31</v>
       </c>
@@ -1070,7 +1070,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>32</v>
       </c>
@@ -1078,7 +1078,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>33</v>
       </c>
@@ -1086,7 +1086,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>34</v>
       </c>
@@ -1094,7 +1094,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>35</v>
       </c>
@@ -1102,7 +1102,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>36</v>
       </c>
@@ -1110,7 +1110,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>37</v>
       </c>
@@ -1118,7 +1118,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>38</v>
       </c>
@@ -1126,7 +1126,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>39</v>
       </c>
@@ -1134,7 +1134,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>40</v>
       </c>
@@ -1142,7 +1142,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>41</v>
       </c>
@@ -1150,7 +1150,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>42</v>
       </c>
@@ -1158,7 +1158,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>131</v>
       </c>
@@ -1166,7 +1166,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>44</v>
       </c>
@@ -1174,7 +1174,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>45</v>
       </c>
@@ -1182,7 +1182,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>46</v>
       </c>
@@ -1190,7 +1190,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>47</v>
       </c>
@@ -1198,7 +1198,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>48</v>
       </c>
@@ -1206,7 +1206,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>49</v>
       </c>
@@ -1214,7 +1214,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>50</v>
       </c>
@@ -1222,7 +1222,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>51</v>
       </c>
@@ -1230,7 +1230,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>52</v>
       </c>
@@ -1238,7 +1238,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>53</v>
       </c>
@@ -1246,7 +1246,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>132</v>
       </c>
@@ -1254,7 +1254,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>55</v>
       </c>
@@ -1262,7 +1262,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>56</v>
       </c>
@@ -1270,7 +1270,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>57</v>
       </c>
@@ -1278,7 +1278,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>58</v>
       </c>
@@ -1286,7 +1286,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>59</v>
       </c>
@@ -1294,7 +1294,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>61</v>
       </c>
@@ -1302,7 +1302,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>62</v>
       </c>
@@ -1310,7 +1310,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>63</v>
       </c>
@@ -1318,7 +1318,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>64</v>
       </c>
@@ -1326,7 +1326,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>65</v>
       </c>
@@ -1334,7 +1334,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>66</v>
       </c>
@@ -1342,7 +1342,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>67</v>
       </c>
@@ -1350,7 +1350,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>68</v>
       </c>
@@ -1358,7 +1358,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>69</v>
       </c>
@@ -1366,7 +1366,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>70</v>
       </c>
@@ -1374,7 +1374,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>71</v>
       </c>
@@ -1382,7 +1382,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>72</v>
       </c>
@@ -1390,7 +1390,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>73</v>
       </c>
@@ -1398,7 +1398,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>74</v>
       </c>
@@ -1406,7 +1406,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>75</v>
       </c>
@@ -1414,7 +1414,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>76</v>
       </c>
@@ -1422,7 +1422,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>77</v>
       </c>
@@ -1430,7 +1430,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>78</v>
       </c>
@@ -1438,7 +1438,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>79</v>
       </c>
@@ -1446,7 +1446,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>80</v>
       </c>
@@ -1454,7 +1454,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>81</v>
       </c>
@@ -1462,7 +1462,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>82</v>
       </c>
@@ -1470,7 +1470,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>83</v>
       </c>
@@ -1478,7 +1478,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>84</v>
       </c>
@@ -1486,7 +1486,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>85</v>
       </c>
@@ -1494,7 +1494,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>86</v>
       </c>
@@ -1502,7 +1502,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>87</v>
       </c>
@@ -1510,7 +1510,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>88</v>
       </c>
@@ -1518,7 +1518,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>89</v>
       </c>
@@ -1526,7 +1526,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>90</v>
       </c>
@@ -1534,7 +1534,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>91</v>
       </c>
@@ -1542,7 +1542,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>92</v>
       </c>
@@ -1550,7 +1550,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>93</v>
       </c>
@@ -1558,7 +1558,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>94</v>
       </c>
@@ -1566,7 +1566,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>95</v>
       </c>
@@ -1574,7 +1574,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>96</v>
       </c>
@@ -1582,7 +1582,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>97</v>
       </c>
@@ -1590,7 +1590,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>98</v>
       </c>
@@ -1598,7 +1598,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>99</v>
       </c>
@@ -1606,7 +1606,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>126</v>
       </c>
@@ -1614,7 +1614,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>101</v>
       </c>
@@ -1622,7 +1622,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>102</v>
       </c>
@@ -1630,7 +1630,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>103</v>
       </c>
@@ -1638,7 +1638,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>104</v>
       </c>
@@ -1646,7 +1646,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>127</v>
       </c>
@@ -1654,7 +1654,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>105</v>
       </c>
@@ -1662,7 +1662,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>106</v>
       </c>
@@ -1670,7 +1670,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>107</v>
       </c>
@@ -1678,7 +1678,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>108</v>
       </c>
@@ -1686,7 +1686,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>109</v>
       </c>
@@ -1694,7 +1694,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>110</v>
       </c>
@@ -1702,7 +1702,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>111</v>
       </c>
@@ -1710,7 +1710,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>112</v>
       </c>
@@ -1718,7 +1718,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>128</v>
       </c>
@@ -1726,7 +1726,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>113</v>
       </c>
@@ -1734,7 +1734,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>114</v>
       </c>
@@ -1742,7 +1742,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>130</v>
       </c>
@@ -1750,7 +1750,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>115</v>
       </c>
@@ -1758,7 +1758,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>129</v>
       </c>
@@ -1766,7 +1766,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>116</v>
       </c>
@@ -1774,7 +1774,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>117</v>
       </c>
@@ -1782,7 +1782,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>118</v>
       </c>
@@ -1790,7 +1790,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>119</v>
       </c>
@@ -1798,7 +1798,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>120</v>
       </c>
@@ -1806,7 +1806,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>121</v>
       </c>
@@ -1814,7 +1814,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>122</v>
       </c>
@@ -1822,7 +1822,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>123</v>
       </c>
@@ -1830,7 +1830,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>124</v>
       </c>

</xml_diff>